<commit_message>
Dungeon fixes and dialog with rogues in altar
</commit_message>
<xml_diff>
--- a/doc/dialog sources/�������� ����� ������/������� ������ ����� ������� ( ���� �� �������� ���� �����).xlsx
+++ b/doc/dialog sources/�������� ����� ������/������� ������ ����� ������� ( ���� �� �������� ���� �����).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="135" windowWidth="19920" windowHeight="7755"/>
@@ -93,8 +93,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +133,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -211,6 +216,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -245,6 +251,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -420,16 +427,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="115" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -437,12 +447,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -450,7 +463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -458,7 +471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -466,7 +479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -474,7 +487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -482,7 +495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -490,7 +503,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -498,7 +511,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -506,7 +519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -514,7 +527,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -522,7 +535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -530,7 +543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -538,7 +551,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -546,7 +559,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
@@ -554,15 +567,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>13</v>
       </c>
       <c r="C17">
         <v>-1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7</v>
       </c>
@@ -570,7 +586,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>16</v>
       </c>
@@ -578,7 +594,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8</v>
       </c>
@@ -586,7 +602,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -594,7 +610,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>19</v>
       </c>
@@ -602,7 +618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9</v>
       </c>
@@ -610,7 +626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -624,24 +640,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>